<commit_message>
Ai Review 27 - 3 - 2025
</commit_message>
<xml_diff>
--- a/Existing AI Model.xlsx
+++ b/Existing AI Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongc\iCloudDrive\2 Study\ Internship\Kidocode\Project - Video Generation AI Modal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongc\iCloudDrive\2 Study\ Internship\Kidocode\Project - AI Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37ED982-B49B-4A83-8F97-5D84CC59DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14350DC8-B363-46C5-83C6-51F46DDFC2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video Generation" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="265">
   <si>
     <t>Model Name</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Token Per Second</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1194,7 @@
   <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95607CB5-2FAD-45D5-8DD5-B8E9322CFB0E}">
-  <dimension ref="B2:G26"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,9 +1833,10 @@
     <col min="5" max="5" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1851,8 +1855,11 @@
       <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>106</v>
       </c>
@@ -1872,7 +1879,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>111</v>
       </c>
@@ -1892,7 +1899,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>114</v>
       </c>
@@ -1912,7 +1919,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>119</v>
       </c>
@@ -1932,7 +1939,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>121</v>
       </c>
@@ -1952,7 +1959,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>124</v>
       </c>
@@ -1972,7 +1979,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>127</v>
       </c>
@@ -1992,7 +1999,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>130</v>
       </c>
@@ -2012,7 +2019,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>133</v>
       </c>
@@ -2032,7 +2039,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>136</v>
       </c>
@@ -2052,7 +2059,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>139</v>
       </c>
@@ -2072,7 +2079,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>142</v>
       </c>
@@ -2092,7 +2099,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>145</v>
       </c>
@@ -2112,7 +2119,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>148</v>
       </c>
@@ -2341,7 +2348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF252098-7689-4A19-BD11-6899AC402416}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>